<commit_message>
refactor verify.py to make it easy to iterate over ODE time step factor and solver tolerances in tests; make _run_test() run a single test, as originally intended; create _run_tests() to iterate over testing parameters; handle tolerances carefully; improve test coverage of testing/verify.py
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/stochastic/00007/00007-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/stochastic/00007/00007-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25520" yWindow="1520" windowWidth="24080" windowHeight="9060" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="-25520" yWindow="1520" windowWidth="24080" windowHeight="9060" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4228,7 +4228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="195">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 16:22:38'</t>
   </si>
@@ -4701,9 +4701,6 @@
     <t>cellular_compartment</t>
   </si>
   <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
     <t>gram</t>
   </si>
   <si>
@@ -4770,9 +4767,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>MW not used</t>
-  </si>
-  <si>
     <t>Sink</t>
   </si>
   <si>
@@ -4816,6 +4810,9 @@
   </si>
   <si>
     <t>mu</t>
+  </si>
+  <si>
+    <t>abstract_compartment</t>
   </si>
 </sst>
 </file>
@@ -5010,18 +5007,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6037,13 +6034,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="28" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6098,22 +6095,22 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6126,22 +6123,22 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6361,21 +6358,21 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6385,21 +6382,21 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -7271,7 +7268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
@@ -7337,7 +7334,7 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -7348,19 +7345,19 @@
         <v>0</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -7371,7 +7368,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -7381,7 +7378,7 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -7392,7 +7389,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -7756,42 +7753,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="28" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="24" t="s">
+      <c r="Q2" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="S2" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="28" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8239,7 +8236,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8257,7 +8254,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -8668,10 +8665,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -9922,7 +9919,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9954,7 +9951,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -9986,7 +9983,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10250,13 +10247,13 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="3"/>
@@ -10382,14 +10379,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.6640625" customWidth="1"/>
+    <col min="1" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="21" width="15.6640625" customWidth="1"/>
     <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10426,29 +10425,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="28" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="28" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10533,15 +10532,15 @@
         <v>156</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -10550,10 +10549,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -10563,7 +10562,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U4" s="3"/>
     </row>
@@ -10788,7 +10787,7 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C4:C13">
       <formula1>"cellular_compartment,extracellular_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D4:D13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D5:D13">
       <formula1>"fluid_compartment,membrane_compartment"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E4:E13">
@@ -10852,7 +10851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
@@ -10884,22 +10883,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="28" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -10955,10 +10954,10 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10971,22 +10970,20 @@
         <v>0</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="M4" s="14"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -10999,14 +10996,12 @@
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="M5" s="14"/>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11228,17 +11223,17 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11248,17 +11243,17 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -11477,23 +11472,23 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="27">
+        <v>180</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="25">
         <v>100</v>
       </c>
       <c r="F3" s="16">
         <v>0</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -11503,23 +11498,23 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="28">
+        <v>181</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="26">
         <v>0</v>
       </c>
       <c r="F4" s="16">
         <v>0</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>

</xml_diff>